<commit_message>
Updated import template with mandatory fields removed
</commit_message>
<xml_diff>
--- a/import-youtube-data-template.xlsx
+++ b/import-youtube-data-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\inhouse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074925E4-CA51-49EF-A88C-D17A422B600C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594EB858-1F55-40A2-B896-55D1EDBACBE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -149,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -161,7 +161,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -171,6 +170,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,41 +454,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19" style="9" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="30.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="14.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="30.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -551,99 +550,99 @@
       <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="W1" s="11" t="s">
         <v>22</v>
       </c>
       <c r="X1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Y1" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated template as per celebrity and brand field added
</commit_message>
<xml_diff>
--- a/import-youtube-data-template.xlsx
+++ b/import-youtube-data-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\inhouse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594EB858-1F55-40A2-B896-55D1EDBACBE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D3960E-ABED-45D1-AEEE-14FCE0F39D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>channel_name</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>name_of_client_worked_before</t>
+  </si>
+  <si>
+    <t>celebrity</t>
+  </si>
+  <si>
+    <t>brands</t>
   </si>
 </sst>
 </file>
@@ -452,7 +458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -486,7 +492,7 @@
     <col min="26" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -562,8 +568,14 @@
       <c r="Y1" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="Z1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
@@ -590,7 +602,7 @@
       <c r="X2" s="6"/>
       <c r="Y2" s="6"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
@@ -617,7 +629,7 @@
       <c r="X3" s="6"/>
       <c r="Y3" s="6"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>

</xml_diff>